<commit_message>
### CsvHelper.OpenXml.Excel feature enhancements
- Refactored ExcelDateTimeOffsetConverter for Excel format conversions;
- Introduced ExcelDateTimeOffsetTextConverter for Excel format conversions;
- Changed CsvHelper.OpenXml.Excel.csproj version, updated to 1.2.0;
- Resolves #1 .

### CsvHelper.OpenXml.Excel.Tests for verifications

- Updated the CsvHelper.OpenXml.Excel.Tests.ConsoleApp console application project to take account of the updates made to the library.
</commit_message>
<xml_diff>
--- a/tests/CsvHelper.OpenXml.Excel.Tests.ConsoleApp/InputTestFiles/CsvHelperOpenXmlInputTest.xlsx
+++ b/tests/CsvHelper.OpenXml.Excel.Tests.ConsoleApp/InputTestFiles/CsvHelperOpenXmlInputTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierl\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0011AE-5BA0-4326-A44F-81E07961BEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F898AD-91F8-4F03-A23B-BC2BFD400E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="1635" windowWidth="31875" windowHeight="29145" activeTab="1" xr2:uid="{E3BD2640-7187-4C88-B208-4DEC019E41BE}"/>
+    <workbookView xWindow="7140" yWindow="5355" windowWidth="36030" windowHeight="24030" xr2:uid="{E3BD2640-7187-4C88-B208-4DEC019E41BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="108">
   <si>
     <t>FirstName</t>
   </si>
@@ -282,19 +282,85 @@
     <t>prova8.pdf</t>
   </si>
   <si>
-    <t>DateTimeOffsetDefault</t>
-  </si>
-  <si>
-    <t>01/01/2024 05:30:00 +02:00</t>
-  </si>
-  <si>
-    <t>02/01/2024 11:00:00 +02:00</t>
-  </si>
-  <si>
-    <t>03/01/2024 12:15:00 +02:00</t>
-  </si>
-  <si>
-    <t>04/01/2024 18:30:00 +02:00</t>
+    <t>01/01/2024 06:30:00+02:00</t>
+  </si>
+  <si>
+    <t>02/01/2024 12:00:00+02:00</t>
+  </si>
+  <si>
+    <t>03/01/2024 13:15:00+02:00</t>
+  </si>
+  <si>
+    <t>04/01/2024 19:30:00+02:00</t>
+  </si>
+  <si>
+    <t>DateTimeOffsetUnspecified</t>
+  </si>
+  <si>
+    <t>DateTimeOffsetUnspecifiedAsText</t>
+  </si>
+  <si>
+    <t>DateTimeOffsetUtc</t>
+  </si>
+  <si>
+    <t>DateTimeOffsetUtcAsText</t>
+  </si>
+  <si>
+    <t>01/01/2024 04:30:00 +00:00</t>
+  </si>
+  <si>
+    <t>02/01/2024 10:00:00 +00:00</t>
+  </si>
+  <si>
+    <t>03/01/2024 11:15:00 +00:00</t>
+  </si>
+  <si>
+    <t>04/01/2024 17:30:00 +00:00</t>
+  </si>
+  <si>
+    <t>01/01/2024 06:30:00 +02:00</t>
+  </si>
+  <si>
+    <t>02/01/2024 12:00:00 +02:00</t>
+  </si>
+  <si>
+    <t>03/01/2024 13:15:00 +02:00</t>
+  </si>
+  <si>
+    <t>04/01/2024 19:30:00 +02:00</t>
+  </si>
+  <si>
+    <t>DateTimeOffsetLocal</t>
+  </si>
+  <si>
+    <t>DateTimeOffsetLocalAsText</t>
+  </si>
+  <si>
+    <t>01/01/2024 05:30:00 +01:00</t>
+  </si>
+  <si>
+    <t>02/01/2024 11:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03/01/2024 12:15:00 +01:00</t>
+  </si>
+  <si>
+    <t>04/01/2024 18:30:00 +01:00</t>
+  </si>
+  <si>
+    <t>DateTimeOffsetUnspecifiedFromDateTimeAsText</t>
+  </si>
+  <si>
+    <t>01/01/2024  08:30:00</t>
+  </si>
+  <si>
+    <t>02/01/2024  14:00:00</t>
+  </si>
+  <si>
+    <t>03/01/2024  15:15:00</t>
+  </si>
+  <si>
+    <t>04/01/2024  21:30:00</t>
   </si>
 </sst>
 </file>
@@ -743,9 +809,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4A3190-BAE5-43FE-9E7F-D4EEE7B49B6C}">
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="34" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF1" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG1" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI1" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ1" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK1" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL1" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4">
+        <v>17</v>
+      </c>
+      <c r="E2" s="23">
+        <v>17.25</v>
+      </c>
+      <c r="F2" s="22">
+        <v>100.25539999999999</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="29">
+        <v>142</v>
+      </c>
+      <c r="K2" s="6">
+        <v>45292</v>
+      </c>
+      <c r="L2" s="21">
+        <v>45292</v>
+      </c>
+      <c r="M2" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>45292</v>
+      </c>
+      <c r="O2" s="8">
+        <v>10</v>
+      </c>
+      <c r="P2" s="9">
+        <v>10.25</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>10.2554</v>
+      </c>
+      <c r="R2" s="25">
+        <v>10.25</v>
+      </c>
+      <c r="S2" s="24">
+        <v>10.2554</v>
+      </c>
+      <c r="T2" s="28">
+        <v>10.25</v>
+      </c>
+      <c r="U2" s="27">
+        <v>10.2554</v>
+      </c>
+      <c r="V2" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="W2" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="X2" s="13">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="Y2" s="14">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="Z2" s="16">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="AA2" s="15">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="AB2" s="17">
+        <v>45292.229166666664</v>
+      </c>
+      <c r="AC2" s="20">
+        <v>45292.229166666664</v>
+      </c>
+      <c r="AD2" s="17">
+        <v>45292.229166666664</v>
+      </c>
+      <c r="AE2" s="20">
+        <v>45292.229166666664</v>
+      </c>
+      <c r="AF2" s="17">
+        <v>45292.3125</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH2" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI2" s="17">
+        <v>45292.1875</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK2" s="17">
+        <v>45292.229166666664</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM2" s="18">
+        <v>100.25</v>
+      </c>
+      <c r="AN2" s="19">
+        <v>100.25539999999999</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4">
+        <v>35</v>
+      </c>
+      <c r="E3" s="23">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="F3" s="22">
+        <v>200.4554</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="29">
+        <v>181</v>
+      </c>
+      <c r="K3" s="6">
+        <v>45293</v>
+      </c>
+      <c r="L3" s="21">
+        <v>45293</v>
+      </c>
+      <c r="M3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
+        <v>45293</v>
+      </c>
+      <c r="O3" s="8">
+        <v>20</v>
+      </c>
+      <c r="P3" s="9">
+        <v>20.45</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>20.455400000000001</v>
+      </c>
+      <c r="R3" s="25">
+        <v>20.45</v>
+      </c>
+      <c r="S3" s="24">
+        <v>20.455400000000001</v>
+      </c>
+      <c r="T3" s="28">
+        <v>20.45</v>
+      </c>
+      <c r="U3" s="27">
+        <v>20.455400000000001</v>
+      </c>
+      <c r="V3" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="W3" s="12">
+        <v>0.105</v>
+      </c>
+      <c r="X3" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="Y3" s="14">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="Z3" s="16">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="AA3" s="15">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="AB3" s="17">
+        <v>45293.458333333336</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>45293.458333333336</v>
+      </c>
+      <c r="AD3" s="17">
+        <v>45293.458333333336</v>
+      </c>
+      <c r="AE3" s="20">
+        <v>45293.458333333336</v>
+      </c>
+      <c r="AF3" s="17">
+        <v>45293.541666666664</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI3" s="17">
+        <v>45293.416666666664</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK3" s="17">
+        <v>45293.458333333336</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM3" s="18">
+        <v>250.45</v>
+      </c>
+      <c r="AN3" s="19">
+        <v>250.4554</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4">
+        <v>55</v>
+      </c>
+      <c r="E4" s="23">
+        <v>55.65</v>
+      </c>
+      <c r="F4" s="22">
+        <v>300.65539999999999</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="29">
+        <v>179</v>
+      </c>
+      <c r="K4" s="6">
+        <v>45294</v>
+      </c>
+      <c r="L4" s="21">
+        <v>45294</v>
+      </c>
+      <c r="M4" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
+        <v>45294</v>
+      </c>
+      <c r="O4" s="8">
+        <v>30</v>
+      </c>
+      <c r="P4" s="9">
+        <v>30.65</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>30.6554</v>
+      </c>
+      <c r="R4" s="25">
+        <v>30.65</v>
+      </c>
+      <c r="S4" s="24">
+        <v>30.6554</v>
+      </c>
+      <c r="T4" s="28">
+        <v>30.65</v>
+      </c>
+      <c r="U4" s="27">
+        <v>30.6554</v>
+      </c>
+      <c r="V4" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="W4" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="X4" s="13">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="Y4" s="14">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="Z4" s="16">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="AA4" s="15">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="AB4" s="17">
+        <v>45294.510416666664</v>
+      </c>
+      <c r="AC4" s="20">
+        <v>45294.510416666664</v>
+      </c>
+      <c r="AD4" s="17">
+        <v>45294.510416666664</v>
+      </c>
+      <c r="AE4" s="20">
+        <v>45294.510416666664</v>
+      </c>
+      <c r="AF4" s="17">
+        <v>45294.59375</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH4" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI4" s="17">
+        <v>45294.46875</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK4" s="17">
+        <v>45294.510416666664</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM4" s="18">
+        <v>3000.65</v>
+      </c>
+      <c r="AN4" s="19">
+        <v>3000.6554000000001</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>51</v>
+      </c>
+      <c r="E5" s="23">
+        <v>51.85</v>
+      </c>
+      <c r="F5" s="22">
+        <v>400.85539999999997</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="29">
+        <v>46</v>
+      </c>
+      <c r="K5" s="6">
+        <v>45295</v>
+      </c>
+      <c r="L5" s="21">
+        <v>45295</v>
+      </c>
+      <c r="M5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>45295</v>
+      </c>
+      <c r="O5" s="8">
+        <v>40</v>
+      </c>
+      <c r="P5" s="9">
+        <v>40.85</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>40.855400000000003</v>
+      </c>
+      <c r="R5" s="25">
+        <v>40.85</v>
+      </c>
+      <c r="S5" s="24">
+        <v>40.855400000000003</v>
+      </c>
+      <c r="T5" s="28">
+        <v>40.85</v>
+      </c>
+      <c r="U5" s="27">
+        <v>40.855400000000003</v>
+      </c>
+      <c r="V5" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="W5" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="X5" s="13">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="Z5" s="16">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="AB5" s="17">
+        <v>45295.770833333336</v>
+      </c>
+      <c r="AC5" s="20">
+        <v>45295.770833333336</v>
+      </c>
+      <c r="AD5" s="17">
+        <v>45295.770833333336</v>
+      </c>
+      <c r="AE5" s="20">
+        <v>45295.770833333336</v>
+      </c>
+      <c r="AF5" s="17">
+        <v>45295.854166666664</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH5" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI5" s="17">
+        <v>45295.729166666664</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK5" s="17">
+        <v>45295.770833333336</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM5" s="18">
+        <v>4768.8500000000004</v>
+      </c>
+      <c r="AN5" s="19">
+        <v>4768.8554000000004</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{4FD33C46-ED4D-47B0-952B-230028BCD451}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{F3B83D78-3431-4429-9E31-EA4C254AD028}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{4A87EEE9-A06B-431E-9BDB-5D28247AA902}"/>
+    <hyperlink ref="H2" r:id="rId4" xr:uid="{2774979E-BDF4-4A2C-ADFD-0F7E9A3FEA9F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60474E8-B61E-4CCA-AF38-CC3124CC1274}">
+  <dimension ref="A1:AO5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -782,13 +1539,17 @@
     <col min="29" max="29" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="34" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -883,27 +1644,45 @@
         <v>39</v>
       </c>
       <c r="AF1" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG1" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI1" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ1" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK1" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL1" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4">
         <v>17</v>
@@ -918,7 +1697,7 @@
         <v>56</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -991,30 +1770,48 @@
         <v>45292.229166666664</v>
       </c>
       <c r="AF2" s="17">
+        <v>45292.3125</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH2" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI2" s="17">
+        <v>45292.1875</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK2" s="17">
         <v>45292.229166666664</v>
       </c>
-      <c r="AG2" s="18">
+      <c r="AL2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM2" s="18">
         <v>100.25</v>
       </c>
-      <c r="AH2" s="19">
+      <c r="AN2" s="19">
         <v>100.25539999999999</v>
       </c>
-      <c r="AI2" t="s">
-        <v>52</v>
+      <c r="AO2" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E3" s="23">
         <v>35.450000000000003</v>
@@ -1026,7 +1823,7 @@
         <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="J3" s="29">
         <v>181</v>
@@ -1074,9 +1871,7 @@
       <c r="X3" s="13">
         <v>0.95833333333333337</v>
       </c>
-      <c r="Y3" s="14">
-        <v>0.95833333333333337</v>
-      </c>
+      <c r="Y3" s="14"/>
       <c r="Z3" s="16">
         <v>0.95833333333333337</v>
       </c>
@@ -1096,30 +1891,48 @@
         <v>45293.458333333336</v>
       </c>
       <c r="AF3" s="17">
+        <v>45293.541666666664</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH3" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI3" s="17">
+        <v>45293.416666666664</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK3" s="17">
         <v>45293.458333333336</v>
       </c>
-      <c r="AG3" s="18">
+      <c r="AL3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM3" s="18">
         <v>250.45</v>
       </c>
-      <c r="AH3" s="19">
+      <c r="AN3" s="19">
         <v>250.4554</v>
       </c>
-      <c r="AI3" t="s">
-        <v>53</v>
+      <c r="AO3" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D4" s="4">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E4" s="23">
         <v>55.65</v>
@@ -1131,7 +1944,7 @@
         <v>58</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="I4" t="s">
         <v>16</v>
@@ -1194,9 +2007,7 @@
       <c r="AB4" s="17">
         <v>45294.510416666664</v>
       </c>
-      <c r="AC4" s="20">
-        <v>45294.510416666664</v>
-      </c>
+      <c r="AC4" s="20"/>
       <c r="AD4" s="17">
         <v>45294.510416666664</v>
       </c>
@@ -1204,30 +2015,48 @@
         <v>45294.510416666664</v>
       </c>
       <c r="AF4" s="17">
+        <v>45294.59375</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH4" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI4" s="17">
+        <v>45294.46875</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK4" s="17">
         <v>45294.510416666664</v>
       </c>
-      <c r="AG4" s="18">
+      <c r="AL4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM4" s="18">
         <v>3000.65</v>
       </c>
-      <c r="AH4" s="19">
+      <c r="AN4" s="19">
         <v>3000.6554000000001</v>
       </c>
-      <c r="AI4" t="s">
-        <v>54</v>
+      <c r="AO4" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="D5" s="4">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E5" s="23">
         <v>51.85</v>
@@ -1236,10 +2065,10 @@
         <v>400.85539999999997</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
         <v>21</v>
@@ -1312,615 +2141,42 @@
         <v>45295.770833333336</v>
       </c>
       <c r="AF5" s="17">
+        <v>45295.854166666664</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH5" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI5" s="17">
+        <v>45295.729166666664</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK5" s="17">
         <v>45295.770833333336</v>
       </c>
-      <c r="AG5" s="18">
+      <c r="AL5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM5" s="18">
         <v>4768.8500000000004</v>
       </c>
-      <c r="AH5" s="19">
-        <v>4768.8554000000004</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>55</v>
+      <c r="AN5" s="19"/>
+      <c r="AO5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{2017B26F-AB62-49C2-916D-D21677D65FE3}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{D321B7BE-49BE-4CF4-8F77-D96D9242FB97}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{AA5A09C8-FBEC-428E-8A39-99B59AF10A52}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{E43AC9B9-6D66-44F1-A1FA-61EB5DA3EC56}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{EE345C7A-3D3F-4875-94A6-FED5A4B85DF7}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{CC439E15-F495-4F63-A300-678B9B1A5D43}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{D450DBBD-4A93-4991-BC70-C19BA3D6E484}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{194D56BD-F031-4CF2-8CDA-A3CFA86CCB21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60474E8-B61E-4CCA-AF38-CC3124CC1274}">
-  <dimension ref="A1:AI5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="34" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF1" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="4">
-        <v>17</v>
-      </c>
-      <c r="E2" s="23">
-        <v>17.25</v>
-      </c>
-      <c r="F2" s="22">
-        <v>100.25539999999999</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="29">
-        <v>142</v>
-      </c>
-      <c r="K2" s="6">
-        <v>45292</v>
-      </c>
-      <c r="L2" s="21">
-        <v>45292</v>
-      </c>
-      <c r="M2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="7">
-        <v>45292</v>
-      </c>
-      <c r="O2" s="8">
-        <v>10</v>
-      </c>
-      <c r="P2" s="9">
-        <v>10.25</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>10.2554</v>
-      </c>
-      <c r="R2" s="25">
-        <v>10.25</v>
-      </c>
-      <c r="S2" s="24">
-        <v>10.2554</v>
-      </c>
-      <c r="T2" s="28">
-        <v>10.25</v>
-      </c>
-      <c r="U2" s="27">
-        <v>10.2554</v>
-      </c>
-      <c r="V2" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="W2" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="X2" s="13">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="Y2" s="14">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="Z2" s="16">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="AA2" s="15">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="AB2" s="17">
-        <v>45292.229166666664</v>
-      </c>
-      <c r="AC2" s="20">
-        <v>45292.229166666664</v>
-      </c>
-      <c r="AD2" s="17">
-        <v>45292.229166666664</v>
-      </c>
-      <c r="AE2" s="20">
-        <v>45292.229166666664</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG2" s="18">
-        <v>100.25</v>
-      </c>
-      <c r="AH2" s="19">
-        <v>100.25539999999999</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="4">
-        <v>30</v>
-      </c>
-      <c r="E3" s="23">
-        <v>35.450000000000003</v>
-      </c>
-      <c r="F3" s="22">
-        <v>200.4554</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="29">
-        <v>181</v>
-      </c>
-      <c r="K3" s="6">
-        <v>45293</v>
-      </c>
-      <c r="L3" s="21">
-        <v>45293</v>
-      </c>
-      <c r="M3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N3" s="7">
-        <v>45293</v>
-      </c>
-      <c r="O3" s="8">
-        <v>20</v>
-      </c>
-      <c r="P3" s="9">
-        <v>20.45</v>
-      </c>
-      <c r="Q3" s="10">
-        <v>20.455400000000001</v>
-      </c>
-      <c r="R3" s="25">
-        <v>20.45</v>
-      </c>
-      <c r="S3" s="24">
-        <v>20.455400000000001</v>
-      </c>
-      <c r="T3" s="28">
-        <v>20.45</v>
-      </c>
-      <c r="U3" s="27">
-        <v>20.455400000000001</v>
-      </c>
-      <c r="V3" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="W3" s="12">
-        <v>0.105</v>
-      </c>
-      <c r="X3" s="13">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="16">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="AA3" s="15">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="AB3" s="17">
-        <v>45293.458333333336</v>
-      </c>
-      <c r="AC3" s="20">
-        <v>45293.458333333336</v>
-      </c>
-      <c r="AD3" s="17">
-        <v>45293.458333333336</v>
-      </c>
-      <c r="AE3" s="20">
-        <v>45293.458333333336</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG3" s="18">
-        <v>250.45</v>
-      </c>
-      <c r="AH3" s="19">
-        <v>250.4554</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="4">
-        <v>28</v>
-      </c>
-      <c r="E4" s="23">
-        <v>55.65</v>
-      </c>
-      <c r="F4" s="22">
-        <v>300.65539999999999</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="29">
-        <v>179</v>
-      </c>
-      <c r="K4" s="6">
-        <v>45294</v>
-      </c>
-      <c r="L4" s="21">
-        <v>45294</v>
-      </c>
-      <c r="M4" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N4" s="7">
-        <v>45294</v>
-      </c>
-      <c r="O4" s="8">
-        <v>30</v>
-      </c>
-      <c r="P4" s="9">
-        <v>30.65</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>30.6554</v>
-      </c>
-      <c r="R4" s="25">
-        <v>30.65</v>
-      </c>
-      <c r="S4" s="24">
-        <v>30.6554</v>
-      </c>
-      <c r="T4" s="28">
-        <v>30.65</v>
-      </c>
-      <c r="U4" s="27">
-        <v>30.6554</v>
-      </c>
-      <c r="V4" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="W4" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="X4" s="13">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="Y4" s="14">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="Z4" s="16">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="AA4" s="15">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="AB4" s="17">
-        <v>45294.510416666664</v>
-      </c>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="17">
-        <v>45294.510416666664</v>
-      </c>
-      <c r="AE4" s="20">
-        <v>45294.510416666664</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG4" s="18">
-        <v>3000.65</v>
-      </c>
-      <c r="AH4" s="19">
-        <v>3000.6554000000001</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="4">
-        <v>62</v>
-      </c>
-      <c r="E5" s="23">
-        <v>51.85</v>
-      </c>
-      <c r="F5" s="22">
-        <v>400.85539999999997</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="29">
-        <v>46</v>
-      </c>
-      <c r="K5" s="6">
-        <v>45295</v>
-      </c>
-      <c r="L5" s="21">
-        <v>45295</v>
-      </c>
-      <c r="M5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>45295</v>
-      </c>
-      <c r="O5" s="8">
-        <v>40</v>
-      </c>
-      <c r="P5" s="9">
-        <v>40.85</v>
-      </c>
-      <c r="Q5" s="10">
-        <v>40.855400000000003</v>
-      </c>
-      <c r="R5" s="25">
-        <v>40.85</v>
-      </c>
-      <c r="S5" s="24">
-        <v>40.855400000000003</v>
-      </c>
-      <c r="T5" s="28">
-        <v>40.85</v>
-      </c>
-      <c r="U5" s="27">
-        <v>40.855400000000003</v>
-      </c>
-      <c r="V5" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="W5" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="X5" s="13">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="Y5" s="14">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="Z5" s="16">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="AA5" s="15">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="AB5" s="17">
-        <v>45295.770833333336</v>
-      </c>
-      <c r="AC5" s="20">
-        <v>45295.770833333336</v>
-      </c>
-      <c r="AD5" s="17">
-        <v>45295.770833333336</v>
-      </c>
-      <c r="AE5" s="20">
-        <v>45295.770833333336</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG5" s="18">
-        <v>4768.8500000000004</v>
-      </c>
-      <c r="AH5" s="19"/>
-      <c r="AI5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{CBEC377B-2109-4EAD-B3C1-539E8963AC59}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{59D46C9E-B5BE-46D9-BB2B-0B60A5F3103B}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{31307EED-5DDF-4F92-AE5D-D2C0A2C663A6}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{9F9EAD26-B68F-40AD-B7D3-86F9B22A5EB1}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>